<commit_message>
Update game statistics data and fix data processing script
- Update raw_data.xlsx with latest game results
- Fix data_processing.py to use correct file paths
- Regenerate ti_data.json with updated statistics
- Move inital_prompt.md to _archive directory

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/raw_data.xlsx
+++ b/data/raw_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Dropbox\Desk\Projects\projects_other\project_ti_auswertung\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642CC615-11A0-43CC-841D-F8DBA1045AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73BF3DB-18D8-4652-955A-73739ED9AC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16356" yWindow="2580" windowWidth="34560" windowHeight="13512" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="120">
   <si>
     <t>game_id</t>
   </si>
@@ -372,6 +372,30 @@
   </si>
   <si>
     <t>Rise and Shine</t>
+  </si>
+  <si>
+    <t>694079731cb455091b9a92cb</t>
+  </si>
+  <si>
+    <t>69505c9be44f36bfafb98b45</t>
+  </si>
+  <si>
+    <t>6962727b1e677f7a6f600b1e</t>
+  </si>
+  <si>
+    <t>696cdb2972af55390d4e54d5</t>
+  </si>
+  <si>
+    <t>TI We verlängert, wenn ihr euch noch in die Augen schauen könnt</t>
+  </si>
+  <si>
+    <t>Jetzt mal ohne Fehler bitte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tommy ist einfach Tommy </t>
+  </si>
+  <si>
+    <t>The return of the Timmy</t>
   </si>
 </sst>
 </file>
@@ -697,21 +721,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+    <sheetView topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114:XFD117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -725,7 +749,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -739,7 +763,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -753,7 +777,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -767,7 +791,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -781,7 +805,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -795,7 +819,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -809,7 +833,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -823,7 +847,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -837,7 +861,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -851,7 +875,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -865,7 +889,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -879,7 +903,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -893,7 +917,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -907,7 +931,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -921,7 +945,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -935,7 +959,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -949,7 +973,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -963,7 +987,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>55</v>
       </c>
@@ -977,7 +1001,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>55</v>
       </c>
@@ -991,7 +1015,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>55</v>
       </c>
@@ -1005,7 +1029,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -1019,7 +1043,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -1033,7 +1057,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -1047,7 +1071,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -1061,7 +1085,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -1075,7 +1099,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -1089,7 +1113,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -1103,7 +1127,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -1117,7 +1141,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -1131,7 +1155,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -1145,7 +1169,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -1159,7 +1183,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -1173,7 +1197,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -1187,7 +1211,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -1201,7 +1225,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>66</v>
       </c>
@@ -1215,7 +1239,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>66</v>
       </c>
@@ -1229,7 +1253,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>66</v>
       </c>
@@ -1243,7 +1267,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>66</v>
       </c>
@@ -1257,7 +1281,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>68</v>
       </c>
@@ -1271,7 +1295,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>68</v>
       </c>
@@ -1285,7 +1309,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>68</v>
       </c>
@@ -1299,7 +1323,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>68</v>
       </c>
@@ -1313,7 +1337,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>70</v>
       </c>
@@ -1327,7 +1351,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -1341,7 +1365,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>70</v>
       </c>
@@ -1355,7 +1379,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>72</v>
       </c>
@@ -1369,7 +1393,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>72</v>
       </c>
@@ -1383,7 +1407,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>72</v>
       </c>
@@ -1397,7 +1421,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>72</v>
       </c>
@@ -1411,7 +1435,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>72</v>
       </c>
@@ -1425,7 +1449,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>74</v>
       </c>
@@ -1439,7 +1463,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>74</v>
       </c>
@@ -1453,7 +1477,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>74</v>
       </c>
@@ -1467,7 +1491,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>76</v>
       </c>
@@ -1481,7 +1505,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>76</v>
       </c>
@@ -1495,7 +1519,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>76</v>
       </c>
@@ -1509,7 +1533,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>78</v>
       </c>
@@ -1523,7 +1547,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>78</v>
       </c>
@@ -1537,7 +1561,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>78</v>
       </c>
@@ -1551,7 +1575,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>78</v>
       </c>
@@ -1565,7 +1589,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>80</v>
       </c>
@@ -1579,7 +1603,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>80</v>
       </c>
@@ -1593,7 +1617,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>80</v>
       </c>
@@ -1607,7 +1631,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>80</v>
       </c>
@@ -1621,7 +1645,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>82</v>
       </c>
@@ -1635,7 +1659,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -1649,7 +1673,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>82</v>
       </c>
@@ -1663,7 +1687,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>83</v>
       </c>
@@ -1677,7 +1701,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>83</v>
       </c>
@@ -1691,7 +1715,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>83</v>
       </c>
@@ -1705,7 +1729,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>85</v>
       </c>
@@ -1719,7 +1743,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -1733,7 +1757,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -1747,7 +1771,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>85</v>
       </c>
@@ -1761,7 +1785,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>87</v>
       </c>
@@ -1775,7 +1799,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>87</v>
       </c>
@@ -1789,7 +1813,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>87</v>
       </c>
@@ -1803,7 +1827,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>89</v>
       </c>
@@ -1817,7 +1841,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>89</v>
       </c>
@@ -1831,7 +1855,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>89</v>
       </c>
@@ -1845,7 +1869,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>89</v>
       </c>
@@ -1859,7 +1883,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -1873,7 +1897,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>91</v>
       </c>
@@ -1887,7 +1911,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -1901,7 +1925,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>93</v>
       </c>
@@ -1915,7 +1939,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>93</v>
       </c>
@@ -1929,7 +1953,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>93</v>
       </c>
@@ -1943,7 +1967,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>93</v>
       </c>
@@ -1957,7 +1981,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>94</v>
       </c>
@@ -1971,7 +1995,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>94</v>
       </c>
@@ -1985,7 +2009,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>94</v>
       </c>
@@ -1999,7 +2023,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>96</v>
       </c>
@@ -2013,7 +2037,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>96</v>
       </c>
@@ -2027,7 +2051,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>96</v>
       </c>
@@ -2041,7 +2065,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>100</v>
       </c>
@@ -2055,7 +2079,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>100</v>
       </c>
@@ -2069,7 +2093,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>100</v>
       </c>
@@ -2083,7 +2107,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>102</v>
       </c>
@@ -2097,7 +2121,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>102</v>
       </c>
@@ -2111,7 +2135,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>102</v>
       </c>
@@ -2125,7 +2149,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>104</v>
       </c>
@@ -2139,7 +2163,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>104</v>
       </c>
@@ -2153,7 +2177,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>104</v>
       </c>
@@ -2167,7 +2191,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>107</v>
       </c>
@@ -2181,7 +2205,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>107</v>
       </c>
@@ -2195,7 +2219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>107</v>
       </c>
@@ -2209,7 +2233,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>109</v>
       </c>
@@ -2223,7 +2247,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>109</v>
       </c>
@@ -2237,7 +2261,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -2251,7 +2275,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -2265,7 +2289,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>110</v>
       </c>
@@ -2279,7 +2303,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>110</v>
       </c>
@@ -2291,6 +2315,188 @@
       </c>
       <c r="D113" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>112</v>
+      </c>
+      <c r="B114" t="s">
+        <v>50</v>
+      </c>
+      <c r="C114">
+        <v>10</v>
+      </c>
+      <c r="D114" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>112</v>
+      </c>
+      <c r="B115" t="s">
+        <v>11</v>
+      </c>
+      <c r="C115">
+        <v>8</v>
+      </c>
+      <c r="D115" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>112</v>
+      </c>
+      <c r="B116" t="s">
+        <v>15</v>
+      </c>
+      <c r="C116">
+        <v>6</v>
+      </c>
+      <c r="D116" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>113</v>
+      </c>
+      <c r="B117" t="s">
+        <v>11</v>
+      </c>
+      <c r="C117">
+        <v>10</v>
+      </c>
+      <c r="D117" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>113</v>
+      </c>
+      <c r="B118" t="s">
+        <v>15</v>
+      </c>
+      <c r="C118">
+        <v>7</v>
+      </c>
+      <c r="D118" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>113</v>
+      </c>
+      <c r="B119" t="s">
+        <v>50</v>
+      </c>
+      <c r="C119">
+        <v>6</v>
+      </c>
+      <c r="D119" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>114</v>
+      </c>
+      <c r="B120" t="s">
+        <v>50</v>
+      </c>
+      <c r="C120">
+        <v>10</v>
+      </c>
+      <c r="D120" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>114</v>
+      </c>
+      <c r="B121" t="s">
+        <v>15</v>
+      </c>
+      <c r="C121">
+        <v>8</v>
+      </c>
+      <c r="D121" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>114</v>
+      </c>
+      <c r="B122" t="s">
+        <v>11</v>
+      </c>
+      <c r="C122">
+        <v>7</v>
+      </c>
+      <c r="D122" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>115</v>
+      </c>
+      <c r="B123" t="s">
+        <v>15</v>
+      </c>
+      <c r="C123">
+        <v>10</v>
+      </c>
+      <c r="D123" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>115</v>
+      </c>
+      <c r="B124" t="s">
+        <v>50</v>
+      </c>
+      <c r="C124">
+        <v>9</v>
+      </c>
+      <c r="D124" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>115</v>
+      </c>
+      <c r="B125" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125">
+        <v>8</v>
+      </c>
+      <c r="D125" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>115</v>
+      </c>
+      <c r="B126" t="s">
+        <v>11</v>
+      </c>
+      <c r="C126">
+        <v>4</v>
+      </c>
+      <c r="D126" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2301,21 +2507,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8F1982-CDD4-4795-9923-90E8136A1DF7}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.88671875" style="1"/>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2335,7 +2541,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2355,7 +2561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -2375,7 +2581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -2395,7 +2601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -2415,7 +2621,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>55</v>
       </c>
@@ -2435,7 +2641,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -2455,7 +2661,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -2475,7 +2681,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -2495,7 +2701,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -2515,7 +2721,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>66</v>
       </c>
@@ -2535,7 +2741,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -2555,7 +2761,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -2575,7 +2781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -2595,7 +2801,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -2615,7 +2821,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -2635,7 +2841,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>78</v>
       </c>
@@ -2655,7 +2861,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -2675,7 +2881,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>82</v>
       </c>
@@ -2695,7 +2901,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -2715,7 +2921,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -2735,7 +2941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -2755,7 +2961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -2775,7 +2981,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>91</v>
       </c>
@@ -2795,7 +3001,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>93</v>
       </c>
@@ -2815,7 +3021,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>94</v>
       </c>
@@ -2835,7 +3041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>96</v>
       </c>
@@ -2855,7 +3061,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>100</v>
       </c>
@@ -2875,7 +3081,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>102</v>
       </c>
@@ -2895,7 +3101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>104</v>
       </c>
@@ -2915,7 +3121,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>107</v>
       </c>
@@ -2935,7 +3141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>109</v>
       </c>
@@ -2955,7 +3161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>110</v>
       </c>
@@ -2972,6 +3178,86 @@
         <v>45959</v>
       </c>
       <c r="F33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34" s="1">
+        <v>46006</v>
+      </c>
+      <c r="E34" s="1">
+        <v>46018</v>
+      </c>
+      <c r="F34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35" s="1">
+        <v>46018</v>
+      </c>
+      <c r="E35" s="1">
+        <v>46032</v>
+      </c>
+      <c r="F35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="D36" s="1">
+        <v>46032</v>
+      </c>
+      <c r="E36" s="1">
+        <v>46037</v>
+      </c>
+      <c r="F36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
+      </c>
+      <c r="D37" s="1">
+        <v>46040</v>
+      </c>
+      <c r="E37" s="1">
+        <v>46055</v>
+      </c>
+      <c r="F37">
         <v>5</v>
       </c>
     </row>
@@ -2988,13 +3274,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -3002,7 +3288,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -3010,7 +3296,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3018,7 +3304,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -3026,7 +3312,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -3034,7 +3320,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -3042,7 +3328,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -3050,7 +3336,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -3058,7 +3344,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -3066,7 +3352,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -3074,7 +3360,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -3082,7 +3368,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -3090,7 +3376,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3098,7 +3384,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -3106,7 +3392,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -3114,7 +3400,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -3122,7 +3408,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -3130,7 +3416,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>44</v>
       </c>

</xml_diff>